<commit_message>
commit dkp and sell docs
</commit_message>
<xml_diff>
--- a/2019_dkp/2019_12_14_dkp.xlsx
+++ b/2019_dkp/2019_12_14_dkp.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Blizzard\World of Warcraft\wow_dkp\2019_dkp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B930ACA-3150-4DCC-8B4F-6D23567CAC2F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27B7A931-5AAC-4483-BC5E-DED12062EC1B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dkp" sheetId="1" r:id="rId1"/>
@@ -656,10 +656,10 @@
   <dimension ref="B1:P60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="E45" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="T51" sqref="T51"/>
+      <selection pane="bottomRight" activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -946,7 +946,10 @@
       <c r="G10" s="7">
         <v>7</v>
       </c>
-      <c r="H10" s="7"/>
+      <c r="H10" s="7">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
       <c r="I10" s="8"/>
       <c r="J10" s="5"/>
       <c r="K10" s="5"/>
@@ -961,7 +964,7 @@
       <c r="O10" s="5"/>
       <c r="P10" s="9">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="2:16" x14ac:dyDescent="0.2">

</xml_diff>